<commit_message>
Updated index and g_ parameters
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\Pipeline_template_CoMaSy\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4545E4-85A5-42ED-B172-37FE65BF4713}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FB263D-9B7C-42CF-8D1C-8DD69E963FE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -331,9 +331,6 @@
     <t>D6_Table_4_IR_ImmDis</t>
   </si>
   <si>
-    <t>D3_clean_spells D3_PERSONS</t>
-  </si>
-  <si>
     <t>D3_persons</t>
   </si>
   <si>
@@ -362,9 +359,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">D3_PERSONS D3_output_spells_category </t>
-  </si>
-  <si>
     <t>MEDICINES EVENTS SURVEY_OBSERVATIONS MEDICAL_OBSERVATIONS</t>
   </si>
   <si>
@@ -416,6 +410,12 @@
   </si>
   <si>
     <t>D5_flowchart_exclusion_criteria D5_flowchart_exclusion_criteria_ImmDis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3_persons D3_output_spells_category </t>
+  </si>
+  <si>
+    <t>D3_clean_spells D3_persons</t>
   </si>
 </sst>
 </file>
@@ -997,7 +997,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,7 +1048,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="7" t="s">
@@ -1109,7 +1109,7 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>18</v>
@@ -1127,13 +1127,13 @@
         <v>10</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="12" t="s">
@@ -1143,13 +1143,13 @@
         <v>10</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="12" t="s">
@@ -1159,13 +1159,13 @@
         <v>26</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12" t="s">
@@ -1175,7 +1175,7 @@
         <v>23</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -1190,12 +1190,12 @@
         <v>70</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>72</v>
@@ -1209,14 +1209,14 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1231,7 +1231,7 @@
         <v>27</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -1249,7 +1249,7 @@
         <v>65</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
         <v>67</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -1616,7 +1616,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1626,18 +1626,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -1888,6 +1876,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1898,23 +1898,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1933,6 +1916,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>

</xml_diff>